<commit_message>
Update prey library energy table to include spiny lobster
</commit_message>
<xml_diff>
--- a/preylib/RawSizeMassData.xlsx
+++ b/preylib/RawSizeMassData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/SOFA2/SOFA/preylib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_BE4698ACE245381CB34A16F4A5252C094C63541B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{80423A54-EE6F-4D3B-8E4B-2896BECA84CA}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_BE4698ACE245381CB34A16F4A5252C094C63541B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E0B51BC2-DA4B-4231-AB2A-D5DE6B1C266D}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="675" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="24150" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RawSizeMassData" sheetId="1" r:id="rId1"/>
@@ -2135,7 +2135,7 @@
   <dimension ref="A1:T2135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1704" sqref="C1704"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>